<commit_message>
Nouvelle répartition des Célestins
</commit_message>
<xml_diff>
--- a/Ferae/Les différents types de Ferae.xlsx
+++ b/Ferae/Les différents types de Ferae.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X181880\OneDrive - GROUP DIGITAL WORKPLACE\Documents\Privé\Ferae\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bertolen\Documents\JdR\Univers\Chroniques des Ténèbres\Ferae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{65500931-93D8-4B88-8DBF-69F84E0A7043}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{3092B04A-39E4-4A87-808A-6F52CD042D96}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A679605C-80A1-46F4-9D59-890BE4D2D201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="4020" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Espèces" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="182">
   <si>
     <t>Espèce</t>
   </si>
@@ -475,7 +477,10 @@
     <t>Férocité</t>
   </si>
   <si>
-    <t>Auspices limitées à Cahalithe et leur Renommé principale est l'Humour</t>
+    <t>Assistance</t>
+  </si>
+  <si>
+    <t>Obéissance</t>
   </si>
   <si>
     <t>Don Exclusif</t>
@@ -526,9 +531,6 @@
     <t>Ravager</t>
   </si>
   <si>
-    <t>Voyager ?</t>
-  </si>
-  <si>
     <t>Voyager, parler</t>
   </si>
   <si>
@@ -583,13 +585,7 @@
     <t>Force</t>
   </si>
   <si>
-    <t>Courage</t>
-  </si>
-  <si>
-    <t>Innovation</t>
-  </si>
-  <si>
-    <t>Harmonie</t>
+    <t>Auspices limitées à Cahalithe et leur Renommé principale est la Ruse</t>
   </si>
 </sst>
 </file>
@@ -659,13 +655,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -675,8 +672,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,28 +952,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.9296875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,27 +988,27 @@
       <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>149</v>
+      <c r="F1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>150</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -1026,18 +1020,18 @@
       <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
@@ -1049,16 +1043,16 @@
       <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="F3" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1069,15 +1063,15 @@
       <c r="E4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F4" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
@@ -1089,21 +1083,21 @@
       <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
@@ -1115,16 +1109,16 @@
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1135,18 +1129,13 @@
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
@@ -1158,18 +1147,18 @@
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>157</v>
+      <c r="F8" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="H8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
@@ -1182,11 +1171,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
@@ -1198,21 +1187,21 @@
       <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C11" t="s">
@@ -1224,18 +1213,18 @@
       <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="F11" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
@@ -1247,21 +1236,18 @@
       <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>162</v>
-      </c>
       <c r="H12" t="s">
         <v>168</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
@@ -1273,31 +1259,25 @@
       <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>167</v>
       </c>
       <c r="H13" t="s">
+        <v>149</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H14" s="4"/>
       <c r="I14" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J13" xr:uid="{34298D81-0FE3-402E-ACB8-ACB4A3B717C7}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Hélios"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J13" xr:uid="{34298D81-0FE3-402E-ACB8-ACB4A3B717C7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1312,12 +1292,12 @@
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1311,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1339,7 +1319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1347,7 +1327,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1355,7 +1335,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1363,7 +1343,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1371,7 +1351,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1379,7 +1359,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1387,7 +1367,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1395,7 +1375,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1403,7 +1383,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +1391,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1419,7 +1399,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1427,7 +1407,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1435,7 +1415,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1446,7 +1426,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1457,7 +1437,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1468,7 +1448,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1479,7 +1459,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1490,7 +1470,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1501,7 +1481,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1512,7 +1492,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1523,7 +1503,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1531,7 +1511,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1539,7 +1519,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1547,7 +1527,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1555,7 +1535,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1563,7 +1543,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1571,7 +1551,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1579,7 +1559,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1587,7 +1567,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1595,7 +1575,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1603,7 +1583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1611,7 +1591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1619,7 +1599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -1627,7 +1607,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1635,7 +1615,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -1643,7 +1623,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -1651,7 +1631,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1659,7 +1639,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -1667,7 +1647,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -1675,7 +1655,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1683,7 +1663,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -1702,22 +1682,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A7BEC1-1CEA-4954-AA1A-91B02B3F1CB1}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="73.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1743,7 +1723,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1753,7 +1733,7 @@
       <c r="C2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="2" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1769,7 +1749,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1779,7 +1759,7 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1795,7 +1775,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1821,7 +1801,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1831,7 +1811,7 @@
       <c r="C5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1847,7 +1827,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1873,7 +1853,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1893,7 +1873,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1903,8 +1883,8 @@
       <c r="C8" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>140</v>
+      <c r="D8" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="E8" t="s">
         <v>58</v>
@@ -1913,7 +1893,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1923,7 +1903,7 @@
       <c r="C9" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>139</v>
       </c>
       <c r="E9" t="s">
@@ -1933,7 +1913,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1943,7 +1923,7 @@
       <c r="C10" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>142</v>
       </c>
       <c r="E10" t="s">
@@ -1953,7 +1933,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1963,9 +1943,7 @@
       <c r="C11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>181</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
         <v>67</v>
       </c>
@@ -1975,7 +1953,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1985,9 +1963,7 @@
       <c r="C12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>140</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
         <v>70</v>
       </c>
@@ -1997,7 +1973,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2007,9 +1983,7 @@
       <c r="C13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>139</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
         <v>73</v>
       </c>
@@ -2019,7 +1993,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -2029,9 +2003,7 @@
       <c r="C14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>182</v>
-      </c>
+      <c r="D14" s="6"/>
       <c r="E14" s="2" t="s">
         <v>76</v>
       </c>
@@ -2041,7 +2013,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -2051,9 +2023,7 @@
       <c r="C15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>142</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
         <v>79</v>
       </c>
@@ -2063,7 +2033,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -2073,9 +2043,7 @@
       <c r="C16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>183</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
         <v>82</v>
       </c>
@@ -2085,7 +2053,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2095,8 +2063,8 @@
       <c r="C17" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>140</v>
+      <c r="D17" t="s">
+        <v>146</v>
       </c>
       <c r="E17" t="s">
         <v>85</v>
@@ -2105,7 +2073,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2115,7 +2083,7 @@
       <c r="C18" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>142</v>
       </c>
       <c r="E18" t="s">
@@ -2125,7 +2093,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2135,8 +2103,8 @@
       <c r="C19" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>139</v>
+      <c r="D19" t="s">
+        <v>141</v>
       </c>
       <c r="E19" t="s">
         <v>91</v>

</xml_diff>